<commit_message>
Integrate Agora data for elec sector variables BECF, BGDPbES, EIaE, EoPPFTSwFP, and FoTCAMRBtPF
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -5,17 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="28680" yWindow="1575" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BGDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -456,51 +464,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -518,15 +528,17 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -639,7 +651,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -787,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -935,303 +947,303 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1379,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1527,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1675,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1823,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1971,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2415,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2563,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2676,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2789,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Update to to model version 3.3.1.1 (including 3.3.1.0)
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257288C8-88AB-4482-B0B3-D67DC1B2D04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1575" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BGDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -111,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,6 +255,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -286,6 +307,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -461,56 +499,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -522,7 +560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -532,13 +570,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.59765625" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -651,7 +689,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -799,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -947,1043 +985,1043 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
         <f t="shared" ref="D9:AK14" si="2">$B9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2131,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2279,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2427,155 +2465,155 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>$B14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2688,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2801,117 +2839,152 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <f>B17</f>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <f t="shared" ref="D17:AK17" si="3">C17</f>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Y17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Z17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AB17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AC17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AD17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AE17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AF17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AG17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AH17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AI17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AJ17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AK17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reduces nuclear power capacity factor & guaranteed dispatch percentage for 2022 to historical data
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257288C8-88AB-4482-B0B3-D67DC1B2D04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516C3C84-5BB4-4FA6-8C09-F05DC3F319C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-53715" yWindow="5175" windowWidth="17415" windowHeight="10290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,9 +220,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,26 +255,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,26 +290,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -502,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -566,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,8 +983,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Electricity sector calibrations. 1) Set geothermal, biomass, and natural gas steam turbine (CHP) to guaranteed dispatch to reflect how these plants operate; 2) Fix assignment issues in start year capacities; 3) Add crude oil plants to economic dispatch; 4) Increase RAF values to 0.9 for technologies less than that; 5) Remove CCS and H2 power plants types from RPS.
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BAB3FF-39B4-48AB-88C4-FD15BF852AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9983F2-56AC-4B15-B13E-A2997E4A2406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Notes:</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>participate in the energy market for extra capacity</t>
+  </si>
+  <si>
+    <t>Natural gas steam turbine (representing CHP), biomass, and geothermal all run at fixed capacity factors, so</t>
+  </si>
+  <si>
+    <t>we flag them here.</t>
   </si>
 </sst>
 </file>
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,6 +711,16 @@
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2501,7 +2517,7 @@
   <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:AK6"/>
+      <selection activeCell="B10" sqref="B10:AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,140 +2757,112 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:R4" si="0">$B3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="J3:AK10" si="1">$B3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -2906,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J3:R4" si="0">$B4</f>
         <v>0</v>
       </c>
       <c r="K4">
@@ -2942,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J3:AK10" si="1">$B4</f>
         <v>0</v>
       </c>
       <c r="T4">
@@ -3699,140 +3687,112 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
-        <f t="shared" ref="G10:AK15" si="2">$B10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -3840,138 +3800,112 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -3983,143 +3917,143 @@
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:I12" si="3">$B12</f>
+        <f t="shared" ref="C12:I12" si="2">$B12</f>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G10:AK15" si="3">$B12</f>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="P12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="R12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="T12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="V12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="W12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="X12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
     </row>
@@ -4143,127 +4077,127 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4296,115 +4230,115 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4440,111 +4374,111 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPS.mdl update to fix capacity factor misalignment; temporary fixes for BGDPbES and TTS to get model running.
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9983F2-56AC-4B15-B13E-A2997E4A2406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B4FD76-34F8-4F64-86D9-7DCCF4757221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="1335" windowWidth="20985" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,7 +2517,7 @@
   <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:AK11"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J3:R4" si="0">$B4</f>
+        <f t="shared" ref="J4:R4" si="0">$B4</f>
         <v>0</v>
       </c>
       <c r="K4">
@@ -2930,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="J3:AK10" si="1">$B4</f>
+        <f t="shared" ref="J4:AK9" si="1">$B4</f>
         <v>0</v>
       </c>
       <c r="T4">
@@ -3913,148 +3913,147 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <f>'Wgtd Avg Expected Cap Factors'!B12</f>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:I12" si="2">$B12</f>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="G10:AK15" si="3">$B12</f>
-        <v>5.6003999999999998E-2</v>
+        <f t="shared" ref="G12:AK15" si="3">$B12</f>
+        <v>0</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="N12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="P12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="R12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="S12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="T12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="U12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="V12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="W12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="X12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="Y12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="Z12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AA12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AB12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AC12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AD12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AE12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AF12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AG12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AH12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AI12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="AK12">
         <f t="shared" si="3"/>
-        <v>5.6003999999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "EPS.mdl update to fix capacity factor misalignment; temporary fixes for BGDPbES and TTS to get model running."
This reverts commit 27f6cfeea7963ae658f1463733f2ec2e49d7aa9d.
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B4FD76-34F8-4F64-86D9-7DCCF4757221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9983F2-56AC-4B15-B13E-A2997E4A2406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="1335" windowWidth="20985" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,7 +2517,7 @@
   <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B10" sqref="B10:AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:R4" si="0">$B4</f>
+        <f t="shared" ref="J3:R4" si="0">$B4</f>
         <v>0</v>
       </c>
       <c r="K4">
@@ -2930,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="J4:AK9" si="1">$B4</f>
+        <f t="shared" ref="J3:AK10" si="1">$B4</f>
         <v>0</v>
       </c>
       <c r="T4">
@@ -3913,147 +3913,148 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <f>'Wgtd Avg Expected Cap Factors'!B12</f>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:I12" si="2">$B12</f>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="G12:AK15" si="3">$B12</f>
-        <v>0</v>
+        <f t="shared" ref="G10:AK15" si="3">$B12</f>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="N12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="P12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="Q12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="R12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="S12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="T12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="U12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="V12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="W12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="X12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="Y12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="Z12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AA12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AB12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AC12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AD12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AE12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AF12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AG12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AH12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AI12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
       <c r="AK12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.6003999999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Electricity sector updates to 1) fix subscript ordering in MPCbS; 2) Update offshore wind capacity to align with latest EU targets; 3) modify electricity parameters to better calibrate the power sector.
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9983F2-56AC-4B15-B13E-A2997E4A2406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB22EFEE-D6CE-418F-9893-BC08D5E85E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14580" yWindow="1620" windowWidth="26730" windowHeight="20460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -611,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -2516,8 +2516,8 @@
   </sheetPr>
   <dimension ref="A1:AK25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:AK11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J3:R4" si="0">$B4</f>
+        <f t="shared" ref="J4:R4" si="0">$B4</f>
         <v>0</v>
       </c>
       <c r="K4">
@@ -2930,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="J3:AK10" si="1">$B4</f>
+        <f t="shared" ref="J4:AK9" si="1">$B4</f>
         <v>0</v>
       </c>
       <c r="T4">
@@ -3264,140 +3264,112 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -3405,140 +3377,112 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -3945,7 +3889,7 @@
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="G10:AK15" si="3">$B12</f>
+        <f t="shared" ref="G12:AK15" si="3">$B12</f>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="K12">
@@ -4347,139 +4291,112 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>